<commit_message>
add new row excell
</commit_message>
<xml_diff>
--- a/application/static/excel_data/data_crawling -- #belajardarirumah.xlsx
+++ b/application/static/excel_data/data_crawling -- #belajardarirumah.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="393">
   <si>
     <t>id</t>
   </si>
@@ -1640,6 +1640,161 @@
   </si>
   <si>
     <t>Tue Dec 08 12:28:05 +0000 2020</t>
+  </si>
+  <si>
+    <t>Selamat Hari Transmigrasi, #GenPrestasi !
+Dimulai sejak tanggal 12 Desember 1950, transmigrasi memiliki tujuan yang melatarbelakangi.
+#IndiHomeStudyByIndiHome #BelajarBarengIndiHomeStudy #BelajarDariRumah #dirumahaja #HariTransmigrasi #Transmigrasi https://t.co/AaNvTXTVSP</t>
+  </si>
+  <si>
+    <t>Sat Dec 12 08:44:45 +0000 2020</t>
+  </si>
+  <si>
+    <t>Kunci Jawaban UAS / PAS Matematika, Kelas 2, Semester Ganjil, Pilihan Ganda &amp;amp; Esai, Berat Buah Jeruk
+#UAS #PAS #PenilaianAkhirSemester #UlanganAkhirSemester #Matematika #belajardirumah #belajardarirumah 
+ https://t.co/i8qHHQEt8B via @tribunkaltim</t>
+  </si>
+  <si>
+    <t>Sat Dec 12 02:07:00 +0000 2020</t>
+  </si>
+  <si>
+    <t>Selamat pagi, #SahabatDikbud. Tayangan-tayangan menarik #BelajardariRumah di @TVRINasional siap hadir untuk menjadi pilihan #SahabatDikbud di akhir pekan. Yuk, simak jadwal acara untuk hari ini, Sabtu, 12 Desember 2020! 
+#MerdekaBelajar
+#BersamaHadapiKorona https://t.co/9FuKr4lokB</t>
+  </si>
+  <si>
+    <t>Sat Dec 12 00:21:07 +0000 2020</t>
+  </si>
+  <si>
+    <t>3. Halo #SahabatPerpusdikbud, saat ini #Perpusdikbud belum melaksanakan layanan tatap muka. Apa yg kalian rindukan dari #Perpusdikbud?
+Ceritakan fasilitas/layanan yg kalian rindukan di kolom komentar&amp;amp; berikan alasannya ya #SahabatPerpusdikbud
+#MerdekaBelajar
+#BelajarDariRumah https://t.co/qTjc83ek4J</t>
+  </si>
+  <si>
+    <t>perpusdikbud</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 23:36:19 +0000 2020</t>
+  </si>
+  <si>
+    <t>2. Halo #SahabatPerpusdikbud, saat ini #Perpusdikbud belum melaksanakan layanan tatap muka. Apa yg kalian rindukan dari #Perpusdikbud?
+Ceritakan fasilitas/layanan yg kalian rindukan di kolom komentar&amp;amp; berikan alasannya ya #SahabatPerpusdikbud
+#MerdekaBelajar
+#BelajarDariRumah https://t.co/pb0xTbct88</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 23:34:57 +0000 2020</t>
+  </si>
+  <si>
+    <t>1. Halo #SahabatPerpusdikbud, saat ini #Perpusdikbud belum melaksanakan layanan tatap muka. Apa yg kalian rindukan dari #Perpusdikbud?
+Ceritakan fasilitas/layanan yg kalian rindukan di kolom komentar&amp;amp; berikan alasannya ya #SahabatPerpusdikbud
+#MerdekaBelajar
+#BelajarDariRumah https://t.co/q76Te8w48f</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 23:33:13 +0000 2020</t>
+  </si>
+  <si>
+    <t>Jadwal Siaran dan Materi Pembelajaran untuk Program "BELAJAR DARI RUMAH" 
+📆 : Sabtu, 12 Desember 2020
+🕗 : 08.00-11.00 WIB 
+🙇‍♀ : Sesuai jenjang pendidikan
+📺 : Panggung Akhir Sekolah Ragam Indonesia pukul 21.30 WIB
+#SemangatBaruMarta
+#BelajarDariRumah
+#MediaPemersatuBangsa https://t.co/6VuMiRcM9c</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 23:00:56 +0000 2020</t>
+  </si>
+  <si>
+    <t>KUNCI JAWABAN Tema 3 Kelas 4 Halaman 126 127 128-130, Ciri-ciri Pertanyaan yang Baik untuk Wawancara
+#BukuTematik #BelajardiRumah #belajardarirumah 
+ https://t.co/gNU3gprcFa via @tribunkaltim</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 21:44:49 +0000 2020</t>
+  </si>
+  <si>
+    <t>Jadwal Siaran dan Materi Pembelajaran untuk Program "BELAJAR DARI RUMAH" 
+📆 : Sabtu, 12 Desember 2020
+🕗 : 08.00-11.00 WIB 
+🙇‍♀ : Sesuai jenjang pendidikan
+📺 : Panggung Akhir Sekolah Ragam Indonesia pukul 21.30 WIB
+#BelajarDariRumah
+#MediaPemersatuBangsa #TVRI #TVRINASIONAL https://t.co/iIccSCjBlB</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 16:18:54 +0000 2020</t>
+  </si>
+  <si>
+    <t>Kadang ada guru/dosen yang memberi tugas di luar batas kemampuan kita sebagai mahasiswa dan manusia biasa, sampe terkadang dalam hati jelek kita sambil sambat "Ya Allah kok tega banget ya, apa sbelumnya gak diukur dulu". Sehat selalu yah pak, bu. #MerdekaBelajar #BelajarDariRumah</t>
+  </si>
+  <si>
+    <t>luthfihr_</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 11:49:27 +0000 2020</t>
+  </si>
+  <si>
+    <t>Kunci Jawaban UAS / PAS Matematika, Kelas 2, Semester Ganjil, Pilihan Ganda  &amp;amp; Esai, Berat Buah Jeruk
+#UAS #PAS #PenilaianAkhirSemester #UlanganAkhirSemester #Matematika #belajardirumah #belajardarirumah 
+https://t.co/i8qHHQW409 via @tribunkaltim</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 03:33:13 +0000 2020</t>
+  </si>
+  <si>
+    <t>Kunci Jawaban UAS / PAS IPA Kelas 7 SMP, Semester Ganjil, Pilihan Ganda, Satuan Besaran yang Dipakai
+#UlanganAkhirSemester #PenilaianAkhirSemester #IPA #belajardirumah #belajardarirumah 
+ https://t.co/Q8Qw67QfI1 via @tribunkaltim</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 02:07:00 +0000 2020</t>
+  </si>
+  <si>
+    <t>Selamat pagi, #SahabatDikbud. Sudah siap untuk belajar hari ini? Jangan lupa siapkan catatanmu, ya! Simak, yuk, jadwal acara #BelajardariRumah di @TVRINasional untuk hari Jumat, 11 Desember 2020! 
+#MerdekaBelajar
+#BersamaHadapiKorona https://t.co/NFkEOfGjwv</t>
+  </si>
+  <si>
+    <t>Fri Dec 11 00:31:51 +0000 2020</t>
+  </si>
+  <si>
+    <t>Jadwal Siaran dan Materi Pembelajaran untuk Program "BELAJAR DARI RUMAH" 
+📆 : Jumat, 11 Desember 2020
+🕗 : 08.00-11.00 WIB 
+🙇‍♀ : Sesuai jenjang pendidikan
+📺 : hanya di TVRI 
+#SemangatBaruMarta
+#BelajarDariRumah
+#MediaPemersatuBangsa #TVRI https://t.co/XjgxgyGVuJ</t>
+  </si>
+  <si>
+    <t>Thu Dec 10 22:19:19 +0000 2020</t>
+  </si>
+  <si>
+    <t>Jadwal Siaran dan Materi Pembelajaran untuk Program "BELAJAR DARI RUMAH" 
+📆 : Jumat, 11 Desember 2020
+🕗 : 08.00-11.00 WIB 
+🙇‍♀ : Sesuai jenjang pendidikan
+📺 : hanya di TVRI 
+#BelajarDariRumah
+#MediaPemersatuBangsa #TVRI #TVRINASIONAL https://t.co/7yIs7EvUyF</t>
+  </si>
+  <si>
+    <t>Thu Dec 10 16:02:24 +0000 2020</t>
+  </si>
+  <si>
+    <t>Segala keputusan panitia bersifat mutlak dan tidak dapat diganggu gugat.
+#digitalinaja #DTSukses #DTSdaring #dirumahaja #belajardarirumah #digiers #digitalent #dts2020 #MakinJagoDigital #SerunyaDTS #digitalinaja⁣ #DTS #DTS2020 #pelatihan⁣ #beasiswa #pelatihangratis</t>
+  </si>
+  <si>
+    <t>DTS_kominfo</t>
+  </si>
+  <si>
+    <t>Thu Dec 10 14:49:53 +0000 2020</t>
   </si>
 </sst>
 </file>
@@ -2004,10 +2159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D156"/>
+  <dimension ref="A1:D175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K147" sqref="K147"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L169" sqref="L169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4196,6 +4351,272 @@
         <v>287</v>
       </c>
     </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>1.337679773883978E+18</v>
+      </c>
+      <c r="B157" t="s">
+        <v>358</v>
+      </c>
+      <c r="C157" t="s">
+        <v>17</v>
+      </c>
+      <c r="D157" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>1.3375796751834399E+18</v>
+      </c>
+      <c r="B158" t="s">
+        <v>360</v>
+      </c>
+      <c r="C158" t="s">
+        <v>26</v>
+      </c>
+      <c r="D158" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>1.337553031802487E+18</v>
+      </c>
+      <c r="B159" t="s">
+        <v>362</v>
+      </c>
+      <c r="C159" t="s">
+        <v>5</v>
+      </c>
+      <c r="D159" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>1.3375417536293361E+18</v>
+      </c>
+      <c r="B160" t="s">
+        <v>364</v>
+      </c>
+      <c r="C160" t="s">
+        <v>365</v>
+      </c>
+      <c r="D160" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>1.3375414106108401E+18</v>
+      </c>
+      <c r="B161" t="s">
+        <v>367</v>
+      </c>
+      <c r="C161" t="s">
+        <v>365</v>
+      </c>
+      <c r="D161" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1.337540973899862E+18</v>
+      </c>
+      <c r="B162" t="s">
+        <v>369</v>
+      </c>
+      <c r="C162" t="s">
+        <v>365</v>
+      </c>
+      <c r="D162" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>1.337532850120212E+18</v>
+      </c>
+      <c r="B163" t="s">
+        <v>371</v>
+      </c>
+      <c r="C163" t="s">
+        <v>8</v>
+      </c>
+      <c r="D163" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>1.337513694964503E+18</v>
+      </c>
+      <c r="B164" t="s">
+        <v>373</v>
+      </c>
+      <c r="C164" t="s">
+        <v>26</v>
+      </c>
+      <c r="D164" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>1.337431673957282E+18</v>
+      </c>
+      <c r="B165" t="s">
+        <v>375</v>
+      </c>
+      <c r="C165" t="s">
+        <v>11</v>
+      </c>
+      <c r="D165" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>1.3373638671946829E+18</v>
+      </c>
+      <c r="B166" t="s">
+        <v>377</v>
+      </c>
+      <c r="C166" t="s">
+        <v>378</v>
+      </c>
+      <c r="D166" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>1.3372389841628239E+18</v>
+      </c>
+      <c r="B167" t="s">
+        <v>380</v>
+      </c>
+      <c r="C167" t="s">
+        <v>26</v>
+      </c>
+      <c r="D167" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>1.337217287330271E+18</v>
+      </c>
+      <c r="B168" t="s">
+        <v>382</v>
+      </c>
+      <c r="C168" t="s">
+        <v>26</v>
+      </c>
+      <c r="D168" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>1.3371933421116421E+18</v>
+      </c>
+      <c r="B169" t="s">
+        <v>384</v>
+      </c>
+      <c r="C169" t="s">
+        <v>5</v>
+      </c>
+      <c r="D169" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>1.3371599905455639E+18</v>
+      </c>
+      <c r="B170" t="s">
+        <v>386</v>
+      </c>
+      <c r="C170" t="s">
+        <v>8</v>
+      </c>
+      <c r="D170" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>1.337065134020309E+18</v>
+      </c>
+      <c r="B171" t="s">
+        <v>388</v>
+      </c>
+      <c r="C171" t="s">
+        <v>11</v>
+      </c>
+      <c r="D171" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>1.3370468871411589E+18</v>
+      </c>
+      <c r="B172" t="s">
+        <v>390</v>
+      </c>
+      <c r="C172" t="s">
+        <v>391</v>
+      </c>
+      <c r="D172" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>1.3368671804329569E+18</v>
+      </c>
+      <c r="B173" t="s">
+        <v>333</v>
+      </c>
+      <c r="C173" t="s">
+        <v>26</v>
+      </c>
+      <c r="D173" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>1.336854899426914E+18</v>
+      </c>
+      <c r="B174" t="s">
+        <v>335</v>
+      </c>
+      <c r="C174" t="s">
+        <v>26</v>
+      </c>
+      <c r="D174" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>1.3368301828548081E+18</v>
+      </c>
+      <c r="B175" t="s">
+        <v>337</v>
+      </c>
+      <c r="C175" t="s">
+        <v>5</v>
+      </c>
+      <c r="D175" t="s">
+        <v>338</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>